<commit_message>
handled the time sync issues
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Document_download_selenium.xlsx
+++ b/src/test/resources/excel/Document_download_selenium.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="180">
   <si>
     <t>Form Name</t>
   </si>
@@ -142,6 +142,438 @@
   </si>
   <si>
     <t>00:06:03</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:40:58</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:41:45</t>
+  </si>
+  <si>
+    <t>00:00:47</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:41:47</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:42:33</t>
+  </si>
+  <si>
+    <t>00:00:46</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:43:20</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:43:21</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:44:08</t>
+  </si>
+  <si>
+    <t>2023-06-29 23:48:50</t>
+  </si>
+  <si>
+    <t>00:04:42</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:25:50</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:02</t>
+  </si>
+  <si>
+    <t>00:00:12</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:07</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:18</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:22</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:34</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:35</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:47</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:26:49</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:27:52</t>
+  </si>
+  <si>
+    <t>00:01:03</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:31:15</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:31:39</t>
+  </si>
+  <si>
+    <t>00:00:24</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:31:41</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:05</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:06</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:30</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:31</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:54</t>
+  </si>
+  <si>
+    <t>00:00:23</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:32:56</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:35:16</t>
+  </si>
+  <si>
+    <t>00:02:20</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:36:28</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:37:05</t>
+  </si>
+  <si>
+    <t>00:00:37</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:37:06</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:37:43</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:37:47</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:38:25</t>
+  </si>
+  <si>
+    <t>00:00:38</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:38:28</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:39:05</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:39:06</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:42:49</t>
+  </si>
+  <si>
+    <t>00:03:43</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:45:12</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:46:14</t>
+  </si>
+  <si>
+    <t>00:01:02</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:46:15</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:47:16</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:47:18</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:48:18</t>
+  </si>
+  <si>
+    <t>00:01:00</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:48:21</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:49:21</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:49:23</t>
+  </si>
+  <si>
+    <t>2023-06-30 00:55:29</t>
+  </si>
+  <si>
+    <t>00:06:06</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:32:35</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:33:37</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:41:37</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:42:39</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:44:25</t>
+  </si>
+  <si>
+    <t>2023-06-30 08:45:26</t>
+  </si>
+  <si>
+    <t>2023-06-30 09:58:56</t>
+  </si>
+  <si>
+    <t>2023-06-30 09:59:57</t>
+  </si>
+  <si>
+    <t>2023-06-30 09:59:58</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:00:58</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:00:59</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:02:00</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:02:01</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:03:02</t>
+  </si>
+  <si>
+    <t>2023-06-30 10:03:03</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:41:14</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:42:17</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:42:19</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:43:20</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:44:26</t>
+  </si>
+  <si>
+    <t>00:01:06</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:44:27</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:45:27</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:45:28</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:51:31</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:58:14</t>
+  </si>
+  <si>
+    <t>2023-06-30 12:59:16</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:01:15</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:02:17</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:04:59</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:06:01</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:06:03</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:07:04</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:07:07</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:08:09</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:08:11</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:09:12</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:09:19</t>
+  </si>
+  <si>
+    <t>2023-06-30 13:15:23</t>
+  </si>
+  <si>
+    <t>00:06:04</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:35:18</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:36:20</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:36:22</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:37:23</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:37:26</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:38:28</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:38:33</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:39:39</t>
+  </si>
+  <si>
+    <t>2023-07-10 23:39:46</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:23:09</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:45:30</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:49:25</t>
+  </si>
+  <si>
+    <t>00:03:55</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:49:27</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:53:22</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:53:24</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:57:19</t>
+  </si>
+  <si>
+    <t>2023-07-11 07:57:20</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:01:15</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:01:17</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:22:25</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:26:24</t>
+  </si>
+  <si>
+    <t>00:03:59</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:26:26</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:30:26</t>
+  </si>
+  <si>
+    <t>00:04:00</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:30:27</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:34:27</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:34:29</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:44:18</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:48:13</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:48:15</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:52:10</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:52:11</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:56:06</t>
+  </si>
+  <si>
+    <t>2023-07-11 08:56:08</t>
+  </si>
+  <si>
+    <t>2023-07-11 09:00:02</t>
+  </si>
+  <si>
+    <t>00:03:54</t>
+  </si>
+  <si>
+    <t>2023-07-11 09:00:04</t>
+  </si>
+  <si>
+    <t>2023-07-11 09:23:32</t>
+  </si>
+  <si>
+    <t>00:23:28</t>
   </si>
 </sst>
 </file>
@@ -545,13 +977,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>24</v>
+        <v>168</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>25</v>
+        <v>169</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>26</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -568,13 +1000,13 @@
         <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>27</v>
+        <v>170</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>26</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -591,13 +1023,13 @@
         <v>13</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>30</v>
+        <v>173</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>26</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -614,13 +1046,13 @@
         <v>13</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>31</v>
+        <v>174</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>32</v>
+        <v>175</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>26</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -637,13 +1069,13 @@
         <v>13</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>33</v>
+        <v>177</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>34</v>
+        <v>178</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>35</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the screen recording in the src/test/resources folder
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Document_download_selenium.xlsx
+++ b/src/test/resources/excel/Document_download_selenium.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="330">
   <si>
     <t>Form Name</t>
   </si>
@@ -982,6 +982,48 @@
   </si>
   <si>
     <t>00:09:48</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:24:03</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:25:36</t>
+  </si>
+  <si>
+    <t>00:01:33</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:25:39</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:27:12</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:27:14</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:28:46</t>
+  </si>
+  <si>
+    <t>00:01:32</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:28:49</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:30:20</t>
+  </si>
+  <si>
+    <t>00:01:31</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:30:23</t>
+  </si>
+  <si>
+    <t>2023-07-12 01:39:36</t>
+  </si>
+  <si>
+    <t>00:09:13</t>
   </si>
 </sst>
 </file>
@@ -1385,13 +1427,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>306</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1408,13 +1450,13 @@
         <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>306</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1431,13 +1473,13 @@
         <v>13</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>306</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1454,13 +1496,13 @@
         <v>13</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>311</v>
+        <v>324</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>306</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1477,13 +1519,13 @@
         <v>13</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>313</v>
+        <v>327</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>314</v>
+        <v>328</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>315</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating with recording of selenium execution
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/Document_download_selenium.xlsx
+++ b/src/test/resources/excel/Document_download_selenium.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="341">
   <si>
     <t>Form Name</t>
   </si>
@@ -1024,6 +1024,39 @@
   </si>
   <si>
     <t>00:09:13</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:50:01</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:51:33</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:51:35</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:53:08</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:53:09</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:54:41</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:54:42</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:56:15</t>
+  </si>
+  <si>
+    <t>2023-07-12 10:56:20</t>
+  </si>
+  <si>
+    <t>2023-07-12 11:05:31</t>
+  </si>
+  <si>
+    <t>00:09:11</t>
   </si>
 </sst>
 </file>
@@ -1427,13 +1460,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>316</v>
+        <v>330</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>317</v>
+        <v>331</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1450,10 +1483,10 @@
         <v>13</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="G3" t="s" s="0">
         <v>318</v>
@@ -1473,10 +1506,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>321</v>
+        <v>334</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>322</v>
+        <v>335</v>
       </c>
       <c r="G4" t="s" s="0">
         <v>323</v>
@@ -1496,13 +1529,13 @@
         <v>13</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1519,13 +1552,13 @@
         <v>13</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>329</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>